<commit_message>
Add Excel-based Inventory Management System with dashboard and stock tracking.
</commit_message>
<xml_diff>
--- a/Inventory Management System.xlsx
+++ b/Inventory Management System.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hirdesh Kumar Yadav\Downloads\Hirdesh Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97CDBD0A-F6C5-4E5D-9C0E-B4D3C453D5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85691655-9E9D-4627-9DDC-E260B249A1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8B51E15A-A4ED-4987-AD62-00E0FD7B820F}"/>
   </bookViews>
@@ -29,11 +29,11 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="161" r:id="rId10"/>
-    <pivotCache cacheId="164" r:id="rId11"/>
-    <pivotCache cacheId="167" r:id="rId12"/>
-    <pivotCache cacheId="171" r:id="rId13"/>
-    <pivotCache cacheId="175" r:id="rId14"/>
+    <pivotCache cacheId="0" r:id="rId10"/>
+    <pivotCache cacheId="1" r:id="rId11"/>
+    <pivotCache cacheId="2" r:id="rId12"/>
+    <pivotCache cacheId="3" r:id="rId13"/>
+    <pivotCache cacheId="4" r:id="rId14"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -492,7 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -510,35 +510,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="48">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -683,6 +662,24 @@
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1079,19 +1076,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:alpha val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -1616,19 +1601,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:alpha val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2048,6 +2021,41 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="50" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN" sz="1800" b="1" i="0" u="none" strike="noStrike" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Stock Available</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IN">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2132,45 +2140,7 @@
           <a:sp3d/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill flip="none" rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1"/>
-                </a:gs>
-                <a:gs pos="75000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                    <a:lumOff val="40000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="51000">
-                  <a:schemeClr val="accent1">
-                    <a:alpha val="75000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="20000"/>
-                    <a:lumOff val="80000"/>
-                    <a:alpha val="15000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:shade val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -16178,105 +16148,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{74C7CA7F-0680-42C4-B048-1D8856EADF80}" name="PivotTable8" cacheId="175" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
-  <location ref="A20:B31" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="8">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="15">
-        <item h="1" x="12"/>
-        <item x="6"/>
-        <item x="3"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="0"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="2"/>
-        <item h="1" x="10"/>
-        <item h="1" x="11"/>
-        <item h="1" x="13"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Stock" fld="5" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="10" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E8B00582-904F-4A66-A742-736CE2E929E1}" name="PivotTable1" cacheId="161" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E8B00582-904F-4A66-A742-736CE2E929E1}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A2:A3" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
@@ -16305,140 +16177,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9137F56D-F959-48FB-9A2F-92C7A05D3F18}" name="PivotTable5" cacheId="175" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A14:A15" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="8">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Stock Amt" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0324D77A-94EF-49E7-8C87-0A9BA903ED56}" name="PivotTable3" cacheId="167" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A8:A9" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Amount" fld="6" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1431EED9-87D1-4669-82F6-6691749C3D3E}" name="PivotTable2" cacheId="164" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A5:A6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="4">
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Product Name" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CA98AEE7-14D6-40AB-96C8-9AAFAB0E64A9}" name="PivotTable4" cacheId="171" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A11:A12" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="9">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Amount" fld="8" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{83D8E7BA-E400-4521-9A6F-0DB0D4F06535}" name="PivotTable7" cacheId="171" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{83D8E7BA-E400-4521-9A6F-0DB0D4F06535}" name="PivotTable7" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
   <location ref="F10:G16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -16533,8 +16273,42 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{39B660B9-1918-4D63-88E2-65EB34C192A6}" name="PivotTable6" cacheId="175" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9137F56D-F959-48FB-9A2F-92C7A05D3F18}" name="PivotTable5" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A14:A15" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="8">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Stock Amt" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{39B660B9-1918-4D63-88E2-65EB34C192A6}" name="PivotTable6" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="12">
   <location ref="F2:G8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -16634,6 +16408,202 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0324D77A-94EF-49E7-8C87-0A9BA903ED56}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A8:A9" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Amount" fld="6" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1431EED9-87D1-4669-82F6-6691749C3D3E}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A5:A6" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Product Name" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CA98AEE7-14D6-40AB-96C8-9AAFAB0E64A9}" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A11:A12" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Amount" fld="8" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{74C7CA7F-0680-42C4-B048-1D8856EADF80}" name="PivotTable8" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13">
+  <location ref="A20:B31" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="15">
+        <item h="1" x="12"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="2"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item h="1" x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Stock" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="10" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4DD6801-6844-48A5-B9D7-3F16A998FCAA}" name="customersdata" displayName="customersdata" ref="D5:G15" totalsRowShown="0" headerRowDxfId="47">
   <autoFilter ref="D5:G15" xr:uid="{C4DD6801-6844-48A5-B9D7-3F16A998FCAA}"/>
@@ -16702,23 +16672,23 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DE1C2028-11E4-4BA1-AEC6-744E20FB8363}" name="salesdata" displayName="salesdata" ref="D5:L23" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="D5:L23" xr:uid="{DE1C2028-11E4-4BA1-AEC6-744E20FB8363}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{15C6E0C3-18FF-4CB8-A9AD-00687A8C7E85}" name="Cust_ID" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{2849888B-F879-4CC4-B1D8-B9F557B7D8C9}" name="Cust_Name" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{15C6E0C3-18FF-4CB8-A9AD-00687A8C7E85}" name="Cust_ID" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{2849888B-F879-4CC4-B1D8-B9F557B7D8C9}" name="Cust_Name" dataDxfId="17">
       <calculatedColumnFormula>IFERROR(VLOOKUP(salesdata[[#This Row],[Cust_ID]],customersdata[#All],2,0),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{72119BB6-F21E-4E86-81E0-F9F9C97EEFD3}" name="HSN Code" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{7C2F278A-D571-4955-B2F6-0A24EF460989}" name="Product Name" dataDxfId="17">
+    <tableColumn id="3" xr3:uid="{72119BB6-F21E-4E86-81E0-F9F9C97EEFD3}" name="HSN Code" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{7C2F278A-D571-4955-B2F6-0A24EF460989}" name="Product Name" dataDxfId="15">
       <calculatedColumnFormula>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],productsdata[#All],2,0),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{DDF17A84-FFC8-4557-A2B3-7C5F76C2F1F0}" name="Date" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{E8BD4F7E-7DE8-48AA-8DE5-DD5ACAD028CB}" name="Stocks(Units)" dataDxfId="15">
+    <tableColumn id="5" xr3:uid="{DDF17A84-FFC8-4557-A2B3-7C5F76C2F1F0}" name="Date" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{E8BD4F7E-7DE8-48AA-8DE5-DD5ACAD028CB}" name="Stocks(Units)" dataDxfId="13">
       <calculatedColumnFormula>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],Table6[#All],6,0),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{1900FEC1-824E-4B81-A776-D1682EB708E1}" name="Units" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{88267E4B-B2C0-4884-8580-62FEF53D7066}" name="Price" dataDxfId="13">
+    <tableColumn id="7" xr3:uid="{1900FEC1-824E-4B81-A776-D1682EB708E1}" name="Units" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{88267E4B-B2C0-4884-8580-62FEF53D7066}" name="Price" dataDxfId="11">
       <calculatedColumnFormula>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],productsdata[#All],4,0),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{DDB1ADCD-B296-4485-9DD2-A7A9702EF7CB}" name="Amount" dataDxfId="12">
+    <tableColumn id="9" xr3:uid="{DDB1ADCD-B296-4485-9DD2-A7A9702EF7CB}" name="Amount" dataDxfId="10">
       <calculatedColumnFormula>IFERROR(salesdata[[#This Row],[Price]]*salesdata[[#This Row],[Units]],"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -16727,31 +16697,31 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{932FD40D-95F8-461A-B450-A833D790AC56}" name="Table6" displayName="Table6" ref="D5:K20" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{932FD40D-95F8-461A-B450-A833D790AC56}" name="Table6" displayName="Table6" ref="D5:K20" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="D5:K20" xr:uid="{932FD40D-95F8-461A-B450-A833D790AC56}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{F38ECE5B-880F-4385-8B13-8CA12CA5429F}" name="HSNCode" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{F38ECE5B-880F-4385-8B13-8CA12CA5429F}" name="HSNCode" dataDxfId="7">
       <calculatedColumnFormula>IFERROR(productsdata[[#This Row],[HSN Code]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{4ACECBC2-19A9-475F-BD54-7367D9E87F54}" name="Product Name" dataDxfId="8">
+    <tableColumn id="2" xr3:uid="{4ACECBC2-19A9-475F-BD54-7367D9E87F54}" name="Product Name" dataDxfId="6">
       <calculatedColumnFormula>IFERROR(productsdata[[#This Row],[Product Name]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5EFEB50F-BDD0-4B73-9863-61EBA0CB3CA8}" name="Cost" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{5EFEB50F-BDD0-4B73-9863-61EBA0CB3CA8}" name="Cost" dataDxfId="5">
       <calculatedColumnFormula>IFERROR(productsdata[[#This Row],[Cost]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{B04F16BA-2529-4D14-8BEF-5ED1540DC4FB}" name="P Units" dataDxfId="6">
+    <tableColumn id="4" xr3:uid="{B04F16BA-2529-4D14-8BEF-5ED1540DC4FB}" name="P Units" dataDxfId="4">
       <calculatedColumnFormula>SUMIF(Table3[Product Name],Table6[[#This Row],[Product Name]],Table3[Units])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{5F24CAB0-BCB3-4613-A68E-2CD3CD521367}" name="S Units" dataDxfId="5">
+    <tableColumn id="5" xr3:uid="{5F24CAB0-BCB3-4613-A68E-2CD3CD521367}" name="S Units" dataDxfId="3">
       <calculatedColumnFormula>SUMIF(salesdata[Product Name],Table6[[#This Row],[Product Name]],salesdata[Units])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{6474EDF5-01CD-411C-9283-EC2DB303DD8D}" name="Stock" dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{6474EDF5-01CD-411C-9283-EC2DB303DD8D}" name="Stock" dataDxfId="2">
       <calculatedColumnFormula>Table6[[#This Row],[P Units]]-Table6[[#This Row],[S Units]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9CFAC6CA-4F46-4A98-91AF-79E56F3B74AE}" name="Stock Amt" dataDxfId="3">
+    <tableColumn id="7" xr3:uid="{9CFAC6CA-4F46-4A98-91AF-79E56F3B74AE}" name="Stock Amt" dataDxfId="1">
       <calculatedColumnFormula>IFERROR(Table6[[#This Row],[Cost]]*Table6[[#This Row],[Stock]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{A8D32168-39F7-4E1F-BABA-ACDD69D8CD94}" name="Notifications" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{A8D32168-39F7-4E1F-BABA-ACDD69D8CD94}" name="Notifications" dataDxfId="0">
       <calculatedColumnFormula>IFERROR(IF(Table6[[#This Row],[Stock]]&lt;5,"📞 "&amp;Table6[[#This Row],[Product Name]]&amp;" Needs to re-order ! PH "&amp; VLOOKUP(Table6[[#This Row],[HSNCode]],Table4[#All],4,0),""),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -17109,7 +17079,7 @@
       <c r="R18" s="12"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="L19" s="14" t="str" cm="1">
+      <c r="L19" s="13" t="str" cm="1">
         <f t="array" ref="L19:L21">_xlfn._xlws.FILTER(Table6[Notifications],Table6[Notifications]&lt;&gt;"")</f>
         <v>📞 Mouse Needs to re-order ! PH 9813xxxxxx</v>
       </c>
@@ -17118,10 +17088,10 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
-      <c r="R19" s="14"/>
+      <c r="R19" s="13"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="L20" s="14" t="str">
+      <c r="L20" s="13" t="str">
         <v>📞 Camera Needs to re-order ! PH 9813xxxxxx</v>
       </c>
       <c r="M20" s="2"/>
@@ -17129,10 +17099,10 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="14"/>
+      <c r="R20" s="13"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="L21" s="14" t="str">
+      <c r="L21" s="13" t="str">
         <v>📞 Headphones Needs to re-order ! PH 9814xxxxxx</v>
       </c>
       <c r="M21" s="2"/>
@@ -17140,19 +17110,19 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
-      <c r="R21" s="14"/>
+      <c r="R21" s="13"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="L22" s="14"/>
+      <c r="L22" s="13"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
-      <c r="R22" s="14"/>
+      <c r="R22" s="13"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="L23" s="14"/>
+      <c r="L23" s="13"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -17161,7 +17131,7 @@
       <c r="R23" s="2"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="L24" s="14"/>
+      <c r="L24" s="13"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -17171,36 +17141,36 @@
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
-      <c r="L25" s="16"/>
+      <c r="L25" s="14"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
-      <c r="L26" s="16"/>
+      <c r="L26" s="14"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
-      <c r="L27" s="16"/>
+      <c r="L27" s="14"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B28" s="1"/>
-      <c r="L28" s="16"/>
+      <c r="L28" s="14"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B29" s="1"/>
-      <c r="L29" s="16"/>
+      <c r="L29" s="14"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B30" s="1"/>
-      <c r="L30" s="16"/>
+      <c r="L30" s="14"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="L31" s="16"/>
+      <c r="L31" s="14"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="L32" s="16"/>
+      <c r="L32" s="14"/>
     </row>
     <row r="33" spans="12:12" x14ac:dyDescent="0.35">
-      <c r="L33" s="16"/>
+      <c r="L33" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17821,7 +17791,7 @@
       <c r="D16" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="1" t="s">
         <v>100</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -17838,7 +17808,7 @@
       <c r="D17" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="1" t="s">
         <v>105</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -18311,11 +18281,11 @@
       <c r="D19" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E19" s="13" t="str">
+      <c r="E19" s="1" t="str">
         <f>IFERROR(VLOOKUP(Table3[[#This Row],[HSN Code]],productsdata[#All],2,0),"")</f>
         <v>Oppo Mobile</v>
       </c>
-      <c r="F19" s="13" t="str">
+      <c r="F19" s="1" t="str">
         <f>IFERROR(VLOOKUP(Table3[[#This Row],[HSN Code]],Table4[#All],3,0),"")</f>
         <v>HR Pvt. Ltd</v>
       </c>
@@ -18325,11 +18295,11 @@
       <c r="H19" s="1">
         <v>40</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="1">
         <f>IFERROR(VLOOKUP(Table3[[#This Row],[HSN Code]],productsdata[#All],3,0),"")</f>
         <v>26999</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J19" s="1">
         <f>IFERROR(Table3[[#This Row],[Units]]*Table3[[#This Row],[Cost]],"")</f>
         <v>1079960</v>
       </c>
@@ -18338,11 +18308,11 @@
       <c r="D20" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E20" s="13" t="str">
+      <c r="E20" s="1" t="str">
         <f>IFERROR(VLOOKUP(Table3[[#This Row],[HSN Code]],productsdata[#All],2,0),"")</f>
         <v>Realme</v>
       </c>
-      <c r="F20" s="13" t="str">
+      <c r="F20" s="1" t="str">
         <f>IFERROR(VLOOKUP(Table3[[#This Row],[HSN Code]],Table4[#All],3,0),"")</f>
         <v>HR Pvt. Ltd</v>
       </c>
@@ -18352,11 +18322,11 @@
       <c r="H20" s="1">
         <v>50</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="1">
         <f>IFERROR(VLOOKUP(Table3[[#This Row],[HSN Code]],productsdata[#All],3,0),"")</f>
         <v>30999</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="1">
         <f>IFERROR(Table3[[#This Row],[Units]]*Table3[[#This Row],[Cost]],"")</f>
         <v>1549950</v>
       </c>
@@ -18847,32 +18817,32 @@
       <c r="D18" s="4">
         <v>102</v>
       </c>
-      <c r="E18" s="13" t="str">
+      <c r="E18" s="1" t="str">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[Cust_ID]],customersdata[#All],2,0),"")</f>
         <v>MK Tech.</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="13" t="str">
+      <c r="G18" s="1" t="str">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],productsdata[#All],2,0),"")</f>
         <v>Mouse</v>
       </c>
       <c r="H18" s="6">
         <v>45332</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18" s="1">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],Table6[#All],6,0),"")</f>
         <v>1</v>
       </c>
       <c r="J18" s="1">
         <v>4</v>
       </c>
-      <c r="K18" s="13">
+      <c r="K18" s="1">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],productsdata[#All],4,0),"")</f>
         <v>240</v>
       </c>
-      <c r="L18" s="13">
+      <c r="L18" s="1">
         <f>IFERROR(salesdata[[#This Row],[Price]]*salesdata[[#This Row],[Units]],"")</f>
         <v>960</v>
       </c>
@@ -18881,32 +18851,32 @@
       <c r="D19" s="4">
         <v>106</v>
       </c>
-      <c r="E19" s="13" t="str">
+      <c r="E19" s="1" t="str">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[Cust_ID]],customersdata[#All],2,0),"")</f>
         <v>jain Tel.</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="13" t="str">
+      <c r="G19" s="1" t="str">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],productsdata[#All],2,0),"")</f>
         <v>Headphones</v>
       </c>
       <c r="H19" s="6">
         <v>41680</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="1">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],Table6[#All],6,0),"")</f>
         <v>2</v>
       </c>
       <c r="J19" s="1">
         <v>6</v>
       </c>
-      <c r="K19" s="13">
+      <c r="K19" s="1">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],productsdata[#All],4,0),"")</f>
         <v>958.8</v>
       </c>
-      <c r="L19" s="13">
+      <c r="L19" s="1">
         <f>IFERROR(salesdata[[#This Row],[Price]]*salesdata[[#This Row],[Units]],"")</f>
         <v>5752.7999999999993</v>
       </c>
@@ -18915,32 +18885,32 @@
       <c r="D20" s="4">
         <v>107</v>
       </c>
-      <c r="E20" s="13" t="str">
+      <c r="E20" s="1" t="str">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[Cust_ID]],customersdata[#All],2,0),"")</f>
         <v>Hirdesh</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G20" s="13" t="str">
+      <c r="G20" s="1" t="str">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],productsdata[#All],2,0),"")</f>
         <v>Oppo Mobile</v>
       </c>
       <c r="H20" s="6">
         <v>45362</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="1">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],Table6[#All],6,0),"")</f>
         <v>30</v>
       </c>
       <c r="J20" s="1">
         <v>10</v>
       </c>
-      <c r="K20" s="13">
+      <c r="K20" s="1">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],productsdata[#All],4,0),"")</f>
         <v>29999</v>
       </c>
-      <c r="L20" s="13">
+      <c r="L20" s="1">
         <f>IFERROR(salesdata[[#This Row],[Price]]*salesdata[[#This Row],[Units]],"")</f>
         <v>299990</v>
       </c>
@@ -18949,32 +18919,32 @@
       <c r="D21" s="4">
         <v>107</v>
       </c>
-      <c r="E21" s="13" t="str">
+      <c r="E21" s="1" t="str">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[Cust_ID]],customersdata[#All],2,0),"")</f>
         <v>Hirdesh</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G21" s="13" t="str">
+      <c r="G21" s="1" t="str">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],productsdata[#All],2,0),"")</f>
         <v>Realme</v>
       </c>
       <c r="H21" s="6">
         <v>45394</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="1">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],Table6[#All],6,0),"")</f>
         <v>5</v>
       </c>
       <c r="J21" s="1">
         <v>25</v>
       </c>
-      <c r="K21" s="13">
+      <c r="K21" s="1">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],productsdata[#All],4,0),"")</f>
         <v>35999</v>
       </c>
-      <c r="L21" s="13">
+      <c r="L21" s="1">
         <f>IFERROR(salesdata[[#This Row],[Price]]*salesdata[[#This Row],[Units]],"")</f>
         <v>899975</v>
       </c>
@@ -18983,32 +18953,32 @@
       <c r="D22" s="4">
         <v>104</v>
       </c>
-      <c r="E22" s="13" t="str">
+      <c r="E22" s="1" t="str">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[Cust_ID]],customersdata[#All],2,0),"")</f>
         <v>Rajesh</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G22" s="13" t="str">
+      <c r="G22" s="1" t="str">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],productsdata[#All],2,0),"")</f>
         <v>Realme</v>
       </c>
       <c r="H22" s="6">
         <v>45395</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="1">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],Table6[#All],6,0),"")</f>
         <v>5</v>
       </c>
       <c r="J22" s="1">
         <v>20</v>
       </c>
-      <c r="K22" s="13">
+      <c r="K22" s="1">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],productsdata[#All],4,0),"")</f>
         <v>35999</v>
       </c>
-      <c r="L22" s="13">
+      <c r="L22" s="1">
         <f>IFERROR(salesdata[[#This Row],[Price]]*salesdata[[#This Row],[Units]],"")</f>
         <v>719980</v>
       </c>
@@ -19017,32 +18987,32 @@
       <c r="D23" s="4">
         <v>107</v>
       </c>
-      <c r="E23" s="13" t="str">
+      <c r="E23" s="1" t="str">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[Cust_ID]],customersdata[#All],2,0),"")</f>
         <v>Hirdesh</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="13" t="str">
+      <c r="G23" s="1" t="str">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],productsdata[#All],2,0),"")</f>
         <v>Desktop</v>
       </c>
       <c r="H23" s="6">
         <v>45425</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="1">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],Table6[#All],6,0),"")</f>
         <v>25</v>
       </c>
       <c r="J23" s="1">
         <v>60</v>
       </c>
-      <c r="K23" s="13">
+      <c r="K23" s="1">
         <f>IFERROR(VLOOKUP(salesdata[[#This Row],[HSN Code]],productsdata[#All],4,0),"")</f>
         <v>25200</v>
       </c>
-      <c r="L23" s="13">
+      <c r="L23" s="1">
         <f>IFERROR(salesdata[[#This Row],[Price]]*salesdata[[#This Row],[Units]],"")</f>
         <v>1512000</v>
       </c>
@@ -19152,7 +19122,7 @@
         <f>IFERROR(Table6[[#This Row],[Cost]]*Table6[[#This Row],[Stock]],"")</f>
         <v>30380</v>
       </c>
-      <c r="K6" s="13" t="str">
+      <c r="K6" s="1" t="str">
         <f>IFERROR(IF(Table6[[#This Row],[Stock]]&lt;5,"📞 "&amp;Table6[[#This Row],[Product Name]]&amp;" Needs to re-order ! PH "&amp; VLOOKUP(Table6[[#This Row],[HSNCode]],Table4[#All],4,0),""),"")</f>
         <v/>
       </c>
@@ -19186,7 +19156,7 @@
         <f>IFERROR(Table6[[#This Row],[Cost]]*Table6[[#This Row],[Stock]],"")</f>
         <v>1621500</v>
       </c>
-      <c r="K7" s="13" t="str">
+      <c r="K7" s="1" t="str">
         <f>IFERROR(IF(Table6[[#This Row],[Stock]]&lt;5,"📞 "&amp;Table6[[#This Row],[Product Name]]&amp;" Needs to re-order ! PH "&amp; VLOOKUP(Table6[[#This Row],[HSNCode]],Table4[#All],4,0),""),"")</f>
         <v/>
       </c>
@@ -19220,7 +19190,7 @@
         <f>IFERROR(Table6[[#This Row],[Cost]]*Table6[[#This Row],[Stock]],"")</f>
         <v>460000</v>
       </c>
-      <c r="K8" s="13" t="str">
+      <c r="K8" s="1" t="str">
         <f>IFERROR(IF(Table6[[#This Row],[Stock]]&lt;5,"📞 "&amp;Table6[[#This Row],[Product Name]]&amp;" Needs to re-order ! PH "&amp; VLOOKUP(Table6[[#This Row],[HSNCode]],Table4[#All],4,0),""),"")</f>
         <v/>
       </c>
@@ -19254,7 +19224,7 @@
         <f>IFERROR(Table6[[#This Row],[Cost]]*Table6[[#This Row],[Stock]],"")</f>
         <v>525000</v>
       </c>
-      <c r="K9" s="13" t="str">
+      <c r="K9" s="1" t="str">
         <f>IFERROR(IF(Table6[[#This Row],[Stock]]&lt;5,"📞 "&amp;Table6[[#This Row],[Product Name]]&amp;" Needs to re-order ! PH "&amp; VLOOKUP(Table6[[#This Row],[HSNCode]],Table4[#All],4,0),""),"")</f>
         <v/>
       </c>
@@ -19288,7 +19258,7 @@
         <f>IFERROR(Table6[[#This Row],[Cost]]*Table6[[#This Row],[Stock]],"")</f>
         <v>200</v>
       </c>
-      <c r="K10" s="13" t="str">
+      <c r="K10" s="1" t="str">
         <f>IFERROR(IF(Table6[[#This Row],[Stock]]&lt;5,"📞 "&amp;Table6[[#This Row],[Product Name]]&amp;" Needs to re-order ! PH "&amp; VLOOKUP(Table6[[#This Row],[HSNCode]],Table4[#All],4,0),""),"")</f>
         <v>📞 Mouse Needs to re-order ! PH 9813xxxxxx</v>
       </c>
@@ -19322,7 +19292,7 @@
         <f>IFERROR(Table6[[#This Row],[Cost]]*Table6[[#This Row],[Stock]],"")</f>
         <v>10200</v>
       </c>
-      <c r="K11" s="13" t="str">
+      <c r="K11" s="1" t="str">
         <f>IFERROR(IF(Table6[[#This Row],[Stock]]&lt;5,"📞 "&amp;Table6[[#This Row],[Product Name]]&amp;" Needs to re-order ! PH "&amp; VLOOKUP(Table6[[#This Row],[HSNCode]],Table4[#All],4,0),""),"")</f>
         <v/>
       </c>
@@ -19356,7 +19326,7 @@
         <f>IFERROR(Table6[[#This Row],[Cost]]*Table6[[#This Row],[Stock]],"")</f>
         <v>52000</v>
       </c>
-      <c r="K12" s="13" t="str">
+      <c r="K12" s="1" t="str">
         <f>IFERROR(IF(Table6[[#This Row],[Stock]]&lt;5,"📞 "&amp;Table6[[#This Row],[Product Name]]&amp;" Needs to re-order ! PH "&amp; VLOOKUP(Table6[[#This Row],[HSNCode]],Table4[#All],4,0),""),"")</f>
         <v>📞 Camera Needs to re-order ! PH 9813xxxxxx</v>
       </c>
@@ -19390,7 +19360,7 @@
         <f>IFERROR(Table6[[#This Row],[Cost]]*Table6[[#This Row],[Stock]],"")</f>
         <v>1598</v>
       </c>
-      <c r="K13" s="13" t="str">
+      <c r="K13" s="1" t="str">
         <f>IFERROR(IF(Table6[[#This Row],[Stock]]&lt;5,"📞 "&amp;Table6[[#This Row],[Product Name]]&amp;" Needs to re-order ! PH "&amp; VLOOKUP(Table6[[#This Row],[HSNCode]],Table4[#All],4,0),""),"")</f>
         <v>📞 Headphones Needs to re-order ! PH 9814xxxxxx</v>
       </c>
@@ -19424,7 +19394,7 @@
         <f>IFERROR(Table6[[#This Row],[Cost]]*Table6[[#This Row],[Stock]],"")</f>
         <v>17420</v>
       </c>
-      <c r="K14" s="13" t="str">
+      <c r="K14" s="1" t="str">
         <f>IFERROR(IF(Table6[[#This Row],[Stock]]&lt;5,"📞 "&amp;Table6[[#This Row],[Product Name]]&amp;" Needs to re-order ! PH "&amp; VLOOKUP(Table6[[#This Row],[HSNCode]],Table4[#All],4,0),""),"")</f>
         <v/>
       </c>
@@ -19458,7 +19428,7 @@
         <f>IFERROR(Table6[[#This Row],[Cost]]*Table6[[#This Row],[Stock]],"")</f>
         <v>493500</v>
       </c>
-      <c r="K15" s="13" t="str">
+      <c r="K15" s="1" t="str">
         <f>IFERROR(IF(Table6[[#This Row],[Stock]]&lt;5,"📞 "&amp;Table6[[#This Row],[Product Name]]&amp;" Needs to re-order ! PH "&amp; VLOOKUP(Table6[[#This Row],[HSNCode]],Table4[#All],4,0),""),"")</f>
         <v/>
       </c>
@@ -19492,7 +19462,7 @@
         <f>IFERROR(Table6[[#This Row],[Cost]]*Table6[[#This Row],[Stock]],"")</f>
         <v>809970</v>
       </c>
-      <c r="K16" s="13" t="str">
+      <c r="K16" s="1" t="str">
         <f>IFERROR(IF(Table6[[#This Row],[Stock]]&lt;5,"📞 "&amp;Table6[[#This Row],[Product Name]]&amp;" Needs to re-order ! PH "&amp; VLOOKUP(Table6[[#This Row],[HSNCode]],Table4[#All],4,0),""),"")</f>
         <v/>
       </c>
@@ -19526,7 +19496,7 @@
         <f>IFERROR(Table6[[#This Row],[Cost]]*Table6[[#This Row],[Stock]],"")</f>
         <v>154995</v>
       </c>
-      <c r="K17" s="13" t="str">
+      <c r="K17" s="1" t="str">
         <f>IFERROR(IF(Table6[[#This Row],[Stock]]&lt;5,"📞 "&amp;Table6[[#This Row],[Product Name]]&amp;" Needs to re-order ! PH "&amp; VLOOKUP(Table6[[#This Row],[HSNCode]],Table4[#All],4,0),""),"")</f>
         <v/>
       </c>
@@ -19560,7 +19530,7 @@
         <f>IFERROR(Table6[[#This Row],[Cost]]*Table6[[#This Row],[Stock]],"")</f>
         <v/>
       </c>
-      <c r="K18" s="13" t="str">
+      <c r="K18" s="1" t="str">
         <f>IFERROR(IF(Table6[[#This Row],[Stock]]&lt;5,"📞 "&amp;Table6[[#This Row],[Product Name]]&amp;" Needs to re-order ! PH "&amp; VLOOKUP(Table6[[#This Row],[HSNCode]],Table4[#All],4,0),""),"")</f>
         <v/>
       </c>
@@ -19582,7 +19552,7 @@
         <f>IFERROR(Table6[[#This Row],[Cost]]*Table6[[#This Row],[Stock]],"")</f>
         <v>0</v>
       </c>
-      <c r="K19" s="13" t="str">
+      <c r="K19" s="1" t="str">
         <f>IFERROR(IF(Table6[[#This Row],[Stock]]&lt;5,"📞 "&amp;Table6[[#This Row],[Product Name]]&amp;" Needs to re-order ! PH "&amp; VLOOKUP(Table6[[#This Row],[HSNCode]],Table4[#All],4,0),""),"")</f>
         <v/>
       </c>
@@ -19616,7 +19586,7 @@
         <f>IFERROR(Table6[[#This Row],[Cost]]*Table6[[#This Row],[Stock]],"")</f>
         <v/>
       </c>
-      <c r="K20" s="13" t="str">
+      <c r="K20" s="1" t="str">
         <f>IFERROR(IF(Table6[[#This Row],[Stock]]&lt;5,"📞 "&amp;Table6[[#This Row],[Product Name]]&amp;" Needs to re-order ! PH "&amp; VLOOKUP(Table6[[#This Row],[HSNCode]],Table4[#All],4,0),""),"")</f>
         <v/>
       </c>
@@ -19662,7 +19632,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="15">
+      <c r="A3">
         <v>8</v>
       </c>
       <c r="C3">
@@ -19672,7 +19642,7 @@
       <c r="F3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3">
         <v>65</v>
       </c>
     </row>
@@ -19680,7 +19650,7 @@
       <c r="F4" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4">
         <v>45</v>
       </c>
     </row>
@@ -19694,12 +19664,12 @@
       <c r="F5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="15">
+      <c r="A6">
         <v>12</v>
       </c>
       <c r="C6">
@@ -19709,7 +19679,7 @@
       <c r="F6" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6">
         <v>19</v>
       </c>
     </row>
@@ -19717,7 +19687,7 @@
       <c r="F7" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7">
         <v>18</v>
       </c>
     </row>
@@ -19731,12 +19701,12 @@
       <c r="F8" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8">
         <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="15">
+      <c r="A9">
         <v>7911690</v>
       </c>
       <c r="C9" s="8">
@@ -19762,12 +19732,12 @@
       <c r="F11" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11">
         <v>2711965</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="15">
+      <c r="A12">
         <v>4403923.4000000004</v>
       </c>
       <c r="C12" s="8">
@@ -19777,7 +19747,7 @@
       <c r="F12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12">
         <v>958180</v>
       </c>
     </row>
@@ -19785,7 +19755,7 @@
       <c r="F13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13">
         <v>312000</v>
       </c>
     </row>
@@ -19799,12 +19769,12 @@
       <c r="F14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14">
         <v>255352.8</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="15">
+      <c r="A15">
         <v>4176763</v>
       </c>
       <c r="C15" s="8">
@@ -19814,7 +19784,7 @@
       <c r="F15" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15">
         <v>126960</v>
       </c>
     </row>
@@ -19822,7 +19792,7 @@
       <c r="F16" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16">
         <v>4364457.8</v>
       </c>
     </row>
@@ -19852,7 +19822,7 @@
       <c r="A21" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21">
         <v>1</v>
       </c>
     </row>
@@ -19860,7 +19830,7 @@
       <c r="A22" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22">
         <v>25</v>
       </c>
     </row>
@@ -19868,7 +19838,7 @@
       <c r="A23" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23">
         <v>2</v>
       </c>
     </row>
@@ -19876,7 +19846,7 @@
       <c r="A24" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24">
         <v>47</v>
       </c>
     </row>
@@ -19884,7 +19854,7 @@
       <c r="A25" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25">
         <v>1</v>
       </c>
     </row>
@@ -19892,7 +19862,7 @@
       <c r="A26" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26">
         <v>30</v>
       </c>
     </row>
@@ -19900,7 +19870,7 @@
       <c r="A27" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27">
         <v>31</v>
       </c>
     </row>
@@ -19908,7 +19878,7 @@
       <c r="A28" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28">
         <v>26</v>
       </c>
     </row>
@@ -19916,7 +19886,7 @@
       <c r="A29" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29">
         <v>21</v>
       </c>
     </row>
@@ -19924,7 +19894,7 @@
       <c r="A30" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30">
         <v>100</v>
       </c>
     </row>
@@ -19932,7 +19902,7 @@
       <c r="A31" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31">
         <v>284</v>
       </c>
     </row>

</xml_diff>